<commit_message>
update: normalization e commerce database
</commit_message>
<xml_diff>
--- a/ecommerce-normalization-db.xlsx
+++ b/ecommerce-normalization-db.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivans\Documents\1 Ivan Workspace\02 Ivan\Projects\02 ivsm-ecommerce\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivans\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61F02783-45D5-4F74-8B45-25B68F8C22E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD1820A5-6565-4367-B273-D9DACCC24D9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{52B46F7A-DB98-43B2-BC07-A6DE30234F11}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="112">
   <si>
     <t>E-COMMERCE DATABASE</t>
   </si>
@@ -288,13 +288,97 @@
   </si>
   <si>
     <t>client_id</t>
+  </si>
+  <si>
+    <t>product_id</t>
+  </si>
+  <si>
+    <t>shopping_id</t>
+  </si>
+  <si>
+    <t>Mis favoritos</t>
+  </si>
+  <si>
+    <t>LISTS_PRODUCTS</t>
+  </si>
+  <si>
+    <t>lists_id</t>
+  </si>
+  <si>
+    <t>discount</t>
+  </si>
+  <si>
+    <t>Chocapic</t>
+  </si>
+  <si>
+    <t>Cereales de chocalate</t>
+  </si>
+  <si>
+    <t>COUPONS_PRODUCTS</t>
+  </si>
+  <si>
+    <t>coupons_id</t>
+  </si>
+  <si>
+    <t>region</t>
+  </si>
+  <si>
+    <t>Los Ríos</t>
+  </si>
+  <si>
+    <t>Regions</t>
+  </si>
+  <si>
+    <t>Communes</t>
+  </si>
+  <si>
+    <t>region_id</t>
+  </si>
+  <si>
+    <t>commune_id</t>
+  </si>
+  <si>
+    <t>address_id</t>
+  </si>
+  <si>
+    <t>Shopping_Products</t>
+  </si>
+  <si>
+    <t>order_date</t>
+  </si>
+  <si>
+    <t>order_approved_at</t>
+  </si>
+  <si>
+    <t>order_delivered_carrier_date</t>
+  </si>
+  <si>
+    <t>order_delivered_client_date</t>
+  </si>
+  <si>
+    <t>Orders</t>
+  </si>
+  <si>
+    <t>approved</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>order_in_preparation_date</t>
+  </si>
+  <si>
+    <t>delivered_carrier</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -324,8 +408,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="15">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -410,8 +502,44 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -503,12 +631,36 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -522,19 +674,29 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -870,20 +1032,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD4D95F3-E5EA-4895-85E5-8389CB4146A2}">
-  <dimension ref="B4:AH68"/>
+  <dimension ref="B4:AL179"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="E72" sqref="E72"/>
+    <sheetView tabSelected="1" topLeftCell="A87" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H102" sqref="H102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14.44140625" customWidth="1"/>
-    <col min="3" max="3" width="18.88671875" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" customWidth="1"/>
+    <col min="3" max="3" width="24.33203125" customWidth="1"/>
     <col min="4" max="4" width="22" customWidth="1"/>
-    <col min="5" max="5" width="21.77734375" customWidth="1"/>
+    <col min="5" max="5" width="26.109375" customWidth="1"/>
     <col min="6" max="6" width="30.109375" customWidth="1"/>
-    <col min="7" max="7" width="22.6640625" customWidth="1"/>
+    <col min="7" max="7" width="24.33203125" customWidth="1"/>
     <col min="8" max="8" width="26.33203125" customWidth="1"/>
     <col min="9" max="9" width="28.6640625" customWidth="1"/>
     <col min="10" max="10" width="31" customWidth="1"/>
@@ -891,8 +1053,8 @@
     <col min="12" max="12" width="15.33203125" customWidth="1"/>
     <col min="13" max="13" width="15.109375" customWidth="1"/>
     <col min="14" max="14" width="15.6640625" customWidth="1"/>
-    <col min="15" max="15" width="17.5546875" customWidth="1"/>
-    <col min="16" max="16" width="38.109375" customWidth="1"/>
+    <col min="15" max="15" width="43.5546875" customWidth="1"/>
+    <col min="16" max="16" width="15.77734375" customWidth="1"/>
     <col min="17" max="17" width="13.88671875" customWidth="1"/>
     <col min="18" max="18" width="27.109375" customWidth="1"/>
     <col min="19" max="19" width="17.5546875" customWidth="1"/>
@@ -900,22 +1062,26 @@
     <col min="21" max="21" width="15.33203125" customWidth="1"/>
     <col min="22" max="22" width="17" customWidth="1"/>
     <col min="23" max="23" width="17.77734375" customWidth="1"/>
-    <col min="24" max="24" width="20.33203125" customWidth="1"/>
+    <col min="24" max="24" width="22" customWidth="1"/>
     <col min="25" max="25" width="22.33203125" customWidth="1"/>
     <col min="26" max="26" width="19.44140625" customWidth="1"/>
+    <col min="27" max="27" width="14.6640625" customWidth="1"/>
     <col min="28" max="28" width="14.44140625" customWidth="1"/>
     <col min="29" max="29" width="18.109375" customWidth="1"/>
-    <col min="30" max="30" width="23.6640625" customWidth="1"/>
+    <col min="30" max="30" width="25.33203125" customWidth="1"/>
+    <col min="31" max="31" width="24.88671875" customWidth="1"/>
     <col min="34" max="34" width="12.77734375" customWidth="1"/>
+    <col min="36" max="36" width="18" customWidth="1"/>
+    <col min="38" max="38" width="24.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:34" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:38" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="6" spans="2:34" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:38" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
         <v>28</v>
       </c>
@@ -950,55 +1116,64 @@
         <v>15</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>4</v>
+        <v>94</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q6" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="R6" s="15" t="s">
+      <c r="Q6" s="13" t="s">
         <v>27</v>
       </c>
+      <c r="R6" s="7" t="s">
+        <v>57</v>
+      </c>
       <c r="S6" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="T6" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="U6" s="13" t="s">
+      <c r="T6" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="V6" s="13" t="s">
+      <c r="U6" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="W6" s="13" t="s">
+      <c r="V6" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="X6" s="13" t="s">
+      <c r="W6" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="Y6" s="13" t="s">
+      <c r="X6" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="Z6" s="13" t="s">
+      <c r="Y6" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="AA6" s="13" t="s">
+      <c r="Z6" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="AB6" s="13" t="s">
+      <c r="AA6" s="15" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="7" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="AB6" s="32" t="s">
+        <v>102</v>
+      </c>
+      <c r="AC6" s="32" t="s">
+        <v>103</v>
+      </c>
+      <c r="AD6" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="AE6" s="32" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="2:38" x14ac:dyDescent="0.3">
       <c r="B7" s="4">
         <v>1</v>
       </c>
@@ -1033,60 +1208,69 @@
         <v>23</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>24</v>
+        <v>95</v>
       </c>
       <c r="N7" s="4" t="s">
         <v>25</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="P7" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="Q7" s="6">
+      <c r="P7" s="6">
         <v>45355</v>
       </c>
-      <c r="R7" s="16">
+      <c r="Q7" s="14">
         <v>3</v>
       </c>
+      <c r="R7" s="7">
+        <v>7500</v>
+      </c>
       <c r="S7" s="7">
+        <v>5000</v>
+      </c>
+      <c r="T7" s="7">
+        <v>13300</v>
+      </c>
+      <c r="U7" s="6">
+        <v>45355</v>
+      </c>
+      <c r="V7" s="7">
         <v>7500</v>
       </c>
-      <c r="T7" s="13">
-        <v>5000</v>
-      </c>
-      <c r="U7" s="13">
-        <v>13300</v>
-      </c>
-      <c r="V7" s="6">
+      <c r="W7" s="7">
+        <v>1</v>
+      </c>
+      <c r="X7" s="7">
+        <v>1</v>
+      </c>
+      <c r="Y7" s="7">
+        <v>1</v>
+      </c>
+      <c r="Z7" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA7" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB7" s="6">
         <v>45355</v>
       </c>
-      <c r="W7" s="7">
-        <v>7500</v>
-      </c>
-      <c r="X7" s="13">
-        <v>1</v>
-      </c>
-      <c r="Y7" s="13">
-        <v>1</v>
-      </c>
-      <c r="Z7" s="13">
-        <v>1</v>
-      </c>
-      <c r="AA7" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="AB7" s="7" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" spans="2:34" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="AC7" s="6">
+        <v>45355</v>
+      </c>
+      <c r="AD7" s="6">
+        <v>45356</v>
+      </c>
+      <c r="AE7" s="6">
+        <v>45356</v>
+      </c>
+    </row>
+    <row r="9" spans="2:38" ht="36.6" x14ac:dyDescent="0.7">
       <c r="B9" s="12" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:34" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:38" x14ac:dyDescent="0.3">
       <c r="B11" s="7" t="s">
         <v>29</v>
       </c>
@@ -1102,7 +1286,7 @@
       <c r="F11" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G11" s="13" t="s">
+      <c r="G11" s="7" t="s">
         <v>54</v>
       </c>
       <c r="H11" s="7" t="s">
@@ -1150,42 +1334,54 @@
       <c r="V11" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="W11" s="15" t="s">
+      <c r="W11" s="13" t="s">
         <v>60</v>
       </c>
       <c r="X11" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="Y11" s="13" t="s">
+      <c r="Y11" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="Z11" s="17" t="s">
+      <c r="Z11" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="AA11" s="13" t="s">
+      <c r="AA11" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="AB11" s="13" t="s">
+      <c r="AB11" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="AC11" s="13" t="s">
+      <c r="AC11" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="AD11" s="13" t="s">
+      <c r="AD11" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="AE11" s="13" t="s">
+      <c r="AE11" s="7" t="s">
         <v>65</v>
       </c>
       <c r="AF11" s="7"/>
-      <c r="AG11" s="13" t="s">
+      <c r="AG11" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="AH11" s="13" t="s">
+      <c r="AH11" s="7" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="12" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="AI11" s="32" t="s">
+        <v>102</v>
+      </c>
+      <c r="AJ11" s="32" t="s">
+        <v>103</v>
+      </c>
+      <c r="AK11" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="AL11" s="32" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="12" spans="2:38" x14ac:dyDescent="0.3">
       <c r="B12" s="7">
         <v>1</v>
       </c>
@@ -1249,16 +1445,16 @@
       <c r="V12" s="6">
         <v>45355</v>
       </c>
-      <c r="W12" s="16">
+      <c r="W12" s="14">
         <v>3</v>
       </c>
       <c r="X12" s="7">
         <v>7500</v>
       </c>
-      <c r="Y12" s="13">
+      <c r="Y12" s="7">
         <v>5000</v>
       </c>
-      <c r="Z12" s="17">
+      <c r="Z12" s="15">
         <v>13300</v>
       </c>
       <c r="AA12" s="9">
@@ -1267,13 +1463,13 @@
       <c r="AB12" s="7">
         <v>7500</v>
       </c>
-      <c r="AC12" s="13">
-        <v>1</v>
-      </c>
-      <c r="AD12" s="13">
-        <v>1</v>
-      </c>
-      <c r="AE12" s="13">
+      <c r="AC12" s="7">
+        <v>1</v>
+      </c>
+      <c r="AD12" s="7">
+        <v>1</v>
+      </c>
+      <c r="AE12" s="7">
         <v>1</v>
       </c>
       <c r="AF12" s="7"/>
@@ -1283,18 +1479,30 @@
       <c r="AH12" s="7" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="14" spans="2:34" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="AI12" s="6">
+        <v>45355</v>
+      </c>
+      <c r="AJ12" s="6">
+        <v>45355</v>
+      </c>
+      <c r="AK12" s="6">
+        <v>45356</v>
+      </c>
+      <c r="AL12" s="6">
+        <v>45356</v>
+      </c>
+    </row>
+    <row r="14" spans="2:38" ht="36.6" x14ac:dyDescent="0.7">
       <c r="B14" s="11" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="2:34" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:38" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B17" s="7" t="s">
         <v>48</v>
       </c>
@@ -1310,11 +1518,11 @@
       <c r="F17" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="G17" s="13" t="s">
+      <c r="G17" s="7" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B18" s="7">
         <v>1</v>
       </c>
@@ -1334,12 +1542,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B21" s="10" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B22" s="7" t="s">
         <v>48</v>
       </c>
@@ -1368,25 +1576,22 @@
         <v>35</v>
       </c>
       <c r="K22" s="7" t="s">
-        <v>4</v>
+        <v>94</v>
       </c>
       <c r="L22" s="7" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="M22" s="7" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="N22" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="O22" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="P22" s="7" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B23" s="7">
         <v>1</v>
       </c>
@@ -1415,30 +1620,27 @@
         <v>23</v>
       </c>
       <c r="K23" s="7" t="s">
-        <v>24</v>
+        <v>95</v>
       </c>
       <c r="L23" s="7" t="s">
         <v>25</v>
       </c>
       <c r="M23" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="N23" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="O23" s="7">
+      <c r="N23" s="7">
         <v>1147</v>
       </c>
-      <c r="P23" s="7" t="s">
+      <c r="O23" s="7" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B26" s="18" t="s">
+    <row r="26" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B26" s="16" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="27" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B27" s="7" t="s">
         <v>48</v>
       </c>
@@ -1451,14 +1653,14 @@
       <c r="E27" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="F27" s="13" t="s">
+      <c r="F27" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="G27" s="13" t="s">
+      <c r="G27" s="7" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="28" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B28" s="7">
         <v>1</v>
       </c>
@@ -1471,359 +1673,841 @@
       <c r="E28" s="7">
         <v>7500</v>
       </c>
-      <c r="F28" s="13">
+      <c r="F28" s="7">
         <v>5000</v>
       </c>
-      <c r="G28" s="13">
+      <c r="G28" s="7">
         <v>13300</v>
       </c>
     </row>
-    <row r="30" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B30" s="19" t="s">
+    <row r="31" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B31" s="33" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="32" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B32" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C32" s="32" t="s">
+        <v>102</v>
+      </c>
+      <c r="D32" s="32" t="s">
+        <v>103</v>
+      </c>
+      <c r="E32" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="F32" s="32" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B33" s="3">
+        <v>1</v>
+      </c>
+      <c r="C33" s="24">
+        <v>45355</v>
+      </c>
+      <c r="D33" s="24">
+        <v>45355</v>
+      </c>
+      <c r="E33" s="24">
+        <v>45356</v>
+      </c>
+      <c r="F33" s="24">
+        <v>45356</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B36" s="17" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="31" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B31" s="7" t="s">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B37" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C31" s="13" t="s">
+      <c r="C37" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="D31" s="13" t="s">
+      <c r="D37" s="7" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="32" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B32" s="7">
-        <v>1</v>
-      </c>
-      <c r="C32" s="9">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B38" s="7">
+        <v>1</v>
+      </c>
+      <c r="C38" s="9">
         <v>45355</v>
       </c>
-      <c r="D32" s="7">
+      <c r="D38" s="7">
         <v>7500</v>
       </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B34" s="20" t="s">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B40" s="18" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B35" s="7" t="s">
+    <row r="41" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B41" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C35" s="13" t="s">
+      <c r="C41" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="D35" s="13" t="s">
+      <c r="D41" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="E35" s="13" t="s">
+      <c r="E41" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="F35" s="14"/>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B36" s="7">
-        <v>1</v>
-      </c>
-      <c r="C36" s="13">
-        <v>1</v>
-      </c>
-      <c r="D36" s="13">
-        <v>1</v>
-      </c>
-      <c r="E36" s="13">
-        <v>1</v>
-      </c>
-      <c r="F36" s="14"/>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B38" s="21" t="s">
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B42" s="7">
+        <v>1</v>
+      </c>
+      <c r="C42" s="7">
+        <v>1</v>
+      </c>
+      <c r="D42" s="7">
+        <v>1</v>
+      </c>
+      <c r="E42" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B44" s="19" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B39" s="7" t="s">
+    <row r="45" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B45" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C39" s="13" t="s">
+      <c r="C45" s="7" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B40" s="7">
-        <v>1</v>
-      </c>
-      <c r="C40" s="7" t="s">
+    <row r="46" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B46" s="7">
+        <v>1</v>
+      </c>
+      <c r="C46" s="7" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B42" s="22" t="s">
+    <row r="48" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B48" s="20" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B43" s="7" t="s">
+    <row r="49" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B49" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C43" s="13" t="s">
+      <c r="C49" s="7" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B44" s="7">
-        <v>1</v>
-      </c>
-      <c r="C44" s="7" t="s">
+    <row r="50" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B50" s="7">
+        <v>1</v>
+      </c>
+      <c r="C50" s="7" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="48" spans="2:6" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="B48" s="23" t="s">
+    <row r="56" spans="2:7" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="B56" s="21" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="51" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B51" s="1" t="s">
+    <row r="59" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B59" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="I51" s="24" t="s">
+    </row>
+    <row r="60" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B60" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D60" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E60" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F60" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G60" s="7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="61" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B61" s="26">
+        <v>1</v>
+      </c>
+      <c r="C61" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="D61" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="E61" s="26">
+        <v>2500</v>
+      </c>
+      <c r="F61" s="26">
+        <v>4</v>
+      </c>
+      <c r="G61" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B62" s="3">
+        <v>2</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E62" s="3">
+        <v>3200</v>
+      </c>
+      <c r="F62" s="3">
+        <v>200</v>
+      </c>
+      <c r="G62" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B65" s="22" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="52" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B52" s="7" t="s">
+    <row r="66" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B66" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C52" s="7" t="s">
+      <c r="C66" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="67" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B67" s="7">
+        <v>1</v>
+      </c>
+      <c r="C67" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="70" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B70" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="71" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B71" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C71" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D52" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="E52" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="F52" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="G52" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="I52" s="7" t="s">
+      <c r="D71" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E71" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F71" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="G71" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="H71" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="I71" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="J71" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="72" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B72" s="7">
+        <v>1</v>
+      </c>
+      <c r="C72" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D72" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E72" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F72" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G72" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H72" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I72" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J72" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="75" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B75" s="23" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="76" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B76" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J52" s="7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="53" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B53" s="7">
-        <v>1</v>
-      </c>
-      <c r="C53" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D53" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="E53" s="7">
-        <v>2500</v>
-      </c>
-      <c r="F53" s="7">
-        <v>4</v>
-      </c>
-      <c r="G53" s="7">
-        <v>1</v>
-      </c>
-      <c r="I53" s="7">
-        <v>1</v>
-      </c>
-      <c r="J53" s="7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="56" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B56" s="10" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="57" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B57" s="7" t="s">
+      <c r="C76" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D76" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E76" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F76" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="G76" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="H76" s="7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="77" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B77" s="7">
+        <v>1</v>
+      </c>
+      <c r="C77" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D77" s="7">
+        <v>1147</v>
+      </c>
+      <c r="E77" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F77" s="7">
+        <v>1</v>
+      </c>
+      <c r="G77" s="7">
+        <v>1</v>
+      </c>
+      <c r="H77" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B80" s="28" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="81" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B81" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C57" s="7" t="s">
+      <c r="C81" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D57" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E57" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F57" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="G57" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="H57" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="I57" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="J57" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="58" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B58" s="7">
-        <v>1</v>
-      </c>
-      <c r="C58" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="D58" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="E58" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="F58" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G58" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="H58" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="I58" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="J58" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="61" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B61" s="25" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="62" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B62" s="7" t="s">
+    </row>
+    <row r="82" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B82" s="3">
+        <v>1</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="85" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B85" s="29" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="86" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B86" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C62" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D62" s="7" t="s">
+      <c r="C86" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D86" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="87" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B87" s="3">
+        <v>1</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D87" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B90" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="91" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B91" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C91" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D91" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E91" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="F91" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="G91" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="H91" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="92" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B92" s="7">
+        <v>1</v>
+      </c>
+      <c r="C92" s="9">
+        <v>45355</v>
+      </c>
+      <c r="D92" s="7">
         <v>3</v>
       </c>
-      <c r="E62" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="F62" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="G62" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="H62" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="I62" s="13" t="s">
+      <c r="E92" s="7">
+        <v>7500</v>
+      </c>
+      <c r="F92" s="7">
+        <v>5000</v>
+      </c>
+      <c r="G92" s="15">
+        <v>13300</v>
+      </c>
+      <c r="H92" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B93" s="7">
+        <v>2</v>
+      </c>
+      <c r="C93" s="9">
+        <v>45355</v>
+      </c>
+      <c r="D93" s="7">
+        <v>2</v>
+      </c>
+      <c r="E93" s="7">
+        <v>6400</v>
+      </c>
+      <c r="F93" s="7">
+        <v>5000</v>
+      </c>
+      <c r="G93" s="15">
+        <v>11400</v>
+      </c>
+      <c r="H93" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B96" s="33" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="97" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B97" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C97" s="32" t="s">
+        <v>102</v>
+      </c>
+      <c r="D97" s="32" t="s">
+        <v>103</v>
+      </c>
+      <c r="E97" s="32" t="s">
+        <v>110</v>
+      </c>
+      <c r="F97" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="G97" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="H97" s="32" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="98" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B98" s="3"/>
+      <c r="C98" s="24">
+        <v>45355</v>
+      </c>
+      <c r="D98" s="24">
+        <v>45355</v>
+      </c>
+      <c r="E98" s="24">
+        <v>45356</v>
+      </c>
+      <c r="F98" s="24">
+        <v>45356</v>
+      </c>
+      <c r="G98" s="24">
+        <v>45356</v>
+      </c>
+      <c r="H98" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B101" s="30" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="102" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B102" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C102" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D102" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="H102" s="31"/>
+    </row>
+    <row r="103" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B103" s="3">
+        <v>1</v>
+      </c>
+      <c r="C103" s="3">
+        <v>1</v>
+      </c>
+      <c r="D103" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B104" s="3">
+        <v>2</v>
+      </c>
+      <c r="C104" s="3">
+        <v>1</v>
+      </c>
+      <c r="D104" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="105" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B105" s="3">
+        <v>3</v>
+      </c>
+      <c r="C105" s="3">
+        <v>2</v>
+      </c>
+      <c r="D105" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="108" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B108" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="G108" s="31"/>
+    </row>
+    <row r="109" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B109" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C109" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D109" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="110" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B110" s="15">
+        <v>1</v>
+      </c>
+      <c r="C110" s="24">
+        <v>45355</v>
+      </c>
+      <c r="D110" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B111" s="15">
+        <v>2</v>
+      </c>
+      <c r="C111" s="24">
+        <v>45356</v>
+      </c>
+      <c r="D111" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="114" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B114" s="18" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="115" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B115" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C115" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="D115" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E115" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="F115" s="32" t="s">
+        <v>111</v>
+      </c>
+      <c r="G115" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="H115" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="I115" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="116" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B116" s="7">
+        <v>1</v>
+      </c>
+      <c r="C116" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="D116" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E116" s="35" t="s">
+        <v>108</v>
+      </c>
+      <c r="F116" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="G116" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="H116" s="3">
+        <v>1</v>
+      </c>
+      <c r="I116" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B117" s="7">
+        <v>1</v>
+      </c>
+      <c r="C117" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="D117" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E117" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="F117" s="32" t="s">
+        <v>109</v>
+      </c>
+      <c r="G117" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="H117" s="3">
+        <v>2</v>
+      </c>
+      <c r="I117" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B120" s="19" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="121" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B121" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C121" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D121" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="63" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B63" s="7">
-        <v>1</v>
-      </c>
-      <c r="C63" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D63" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E63" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F63" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G63" s="7">
-        <v>1147</v>
-      </c>
-      <c r="H63" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="I63" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B66" s="18" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B67" s="7" t="s">
+    <row r="122" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B122" s="3">
+        <v>1</v>
+      </c>
+      <c r="C122" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D122" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B123" s="3">
+        <v>2</v>
+      </c>
+      <c r="C123" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D123" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B126" s="25" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="127" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B127" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C67" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="D67" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="E67" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="F67" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="G67" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="H67" s="13" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B68" s="7">
-        <v>1</v>
-      </c>
-      <c r="C68" s="9">
-        <v>45355</v>
-      </c>
-      <c r="D68" s="7">
-        <v>3</v>
-      </c>
-      <c r="E68" s="7">
-        <v>7500</v>
-      </c>
-      <c r="F68" s="13">
-        <v>5000</v>
-      </c>
-      <c r="G68" s="13">
-        <v>13300</v>
-      </c>
-      <c r="H68" s="13">
-        <v>1</v>
-      </c>
+      <c r="C127" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D127" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="128" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B128" s="3">
+        <v>1</v>
+      </c>
+      <c r="C128" s="3">
+        <v>2</v>
+      </c>
+      <c r="D128" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B129" s="3">
+        <v>2</v>
+      </c>
+      <c r="C129" s="3">
+        <v>2</v>
+      </c>
+      <c r="D129" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="132" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B132" s="20" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="133" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B133" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C133" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="D133" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="134" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B134" s="7">
+        <v>1</v>
+      </c>
+      <c r="C134" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="D134" s="3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="137" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B137" s="27" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="138" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B138" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C138" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D138" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="139" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B139" s="3">
+        <v>1</v>
+      </c>
+      <c r="C139" s="3">
+        <v>1</v>
+      </c>
+      <c r="D139" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="179" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F179" s="31"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="I7" r:id="rId1" xr:uid="{1BA249DE-510C-4A43-858A-CC7621062249}"/>
     <hyperlink ref="L12" r:id="rId2" xr:uid="{155341EB-2B56-45CF-8C29-889C804F9642}"/>
     <hyperlink ref="G23" r:id="rId3" xr:uid="{813B1712-5449-482D-BFAD-B9D6DD1635A9}"/>
-    <hyperlink ref="G58" r:id="rId4" xr:uid="{612F4E5D-CC59-4D46-B63C-D2E001CF0F59}"/>
+    <hyperlink ref="G72" r:id="rId4" xr:uid="{612F4E5D-CC59-4D46-B63C-D2E001CF0F59}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>